<commit_message>
UC 4 e UC 7 - Test Scenarios
</commit_message>
<xml_diff>
--- a/Análise/Test Scenarios - Julio.xlsx
+++ b/Análise/Test Scenarios - Julio.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855"/>
   </bookViews>
   <sheets>
-    <sheet name="UC 4 - " sheetId="1" r:id="rId1"/>
-    <sheet name="Folha2" sheetId="2" r:id="rId2"/>
+    <sheet name="UC 4-Especificar Comp.Técnica " sheetId="1" r:id="rId1"/>
+    <sheet name="UC 7-Publicar Tarefa" sheetId="2" r:id="rId2"/>
     <sheet name="Folha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="91">
   <si>
     <t>Project Name</t>
   </si>
@@ -45,61 +45,27 @@
     <t>Test Scenario Description</t>
   </si>
   <si>
-    <t>Check Registar Organização functionality</t>
-  </si>
-  <si>
     <t>Test Case ID</t>
   </si>
   <si>
     <t>Test Case Description</t>
   </si>
   <si>
-    <t>Valid Org Name
-Valid Org NIF
-Valid Org Email
-Valid Org Website
-Valid Org Phone Number
-Valid Org Address</t>
-  </si>
-  <si>
     <t>Test Case Steps</t>
   </si>
   <si>
-    <t>1. Enter valid org name
-2. Enter valid org nif
-3. Enter valid org email
-4. Enter valid org website
-5. Enter valid org phone number
-6. Enter valid org address
-7. Click register button</t>
-  </si>
-  <si>
     <t>Preconditions</t>
   </si>
   <si>
     <t>Test Data</t>
   </si>
   <si>
-    <t>org name: org123
-org nif: 123456789
-org email: org123@org123.com
-org website: org123.com
-org phone number: 911123123
-org address: rua sousa, 1, 4000-400, Porto</t>
-  </si>
-  <si>
     <t>Post Conditions</t>
   </si>
   <si>
-    <t>Message "Organization successfully registered"</t>
-  </si>
-  <si>
     <t>Expected Result</t>
   </si>
   <si>
-    <t>Successful register of an Organization</t>
-  </si>
-  <si>
     <t>Actual Result</t>
   </si>
   <si>
@@ -128,6 +94,347 @@
   </si>
   <si>
     <t>TC_UC4_004</t>
+  </si>
+  <si>
+    <t>Valid unique code
+Valid brief description
+Valid detailed description
+Valid activity area
+Valid proficiency degrees</t>
+  </si>
+  <si>
+    <t>Message "Technical skill sucefully registered"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique code: CP-01
+brief description: "Pintura Imóveis"
+detailed description: "Pintura interior e exterior de imóveis"
+activity area: "Construção"
+proficiency degrees: 0-5, from 0 for "really bad" to 5 for "master at painting"
+</t>
+  </si>
+  <si>
+    <t>Successful register a technical skill</t>
+  </si>
+  <si>
+    <t>Already existant unique code
+Valid brief description
+Valid detailed description
+Valid activity area
+Valid proficiency degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique code: CP-01
+brief description: "Reparação Automóvel"
+detailed description: "Reparação mecánica automóvel, mecánica geral"
+activity area: "Mecánica"
+proficiency degrees: 0-5, from 0 for "really bad" to 5 for "master at mechanics"
+</t>
+  </si>
+  <si>
+    <t>Message "Unique code already exists"</t>
+  </si>
+  <si>
+    <t>Popup Message "Unique code already exists"</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique code: ###1
+brief description: "Pintura Imóveis"
+detailed description: "Pintura interior e exterior de imóveis"
+activity area: "Construção"
+proficiency degrees: 0-5, from 0 for "really bad" to 5 for "master at painting"
+</t>
+  </si>
+  <si>
+    <t>Message "Invalid unique code"</t>
+  </si>
+  <si>
+    <t>Popup Message "Invalid unique code"</t>
+  </si>
+  <si>
+    <t>TC_UC4_005</t>
+  </si>
+  <si>
+    <t>TC_UC4_006</t>
+  </si>
+  <si>
+    <t>Invalid unique code
+Valid brief description
+Valid detailed description
+Valid activity area
+Valid proficiency degrees</t>
+  </si>
+  <si>
+    <t>Valid unique code
+Invalid brief description
+Valid detailed description
+Valid activity area
+Valid proficiency degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique code: CP-02
+brief description: " "
+detailed description: "Pintura interior e exterior de imóveis"
+activity area: "Construção"
+proficiency degrees: 0-5, from 0 for "really bad" to 5 for "master at painting"
+</t>
+  </si>
+  <si>
+    <t>Message "Invalid brief description"</t>
+  </si>
+  <si>
+    <t>Popup Message "Invalid brief description"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique code: CP-03
+brief description: "Pintura Imóveis"
+detailed description: " "
+activity area: "Construção"
+proficiency degrees: 0-5, from 0 for "really bad" to 5 for "master at painting"
+</t>
+  </si>
+  <si>
+    <t>Message "Invalid detailed description"</t>
+  </si>
+  <si>
+    <t>TC_UC4_007</t>
+  </si>
+  <si>
+    <t>Valid unique code
+Valid brief description
+Invalid detailed description
+Valid activity area
+Valid proficiency degrees</t>
+  </si>
+  <si>
+    <t>Valid unique code
+Valid brief description
+Valid detailed description
+Invalid activity area
+Valid proficiency degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique code: CP-04
+brief description: "Pintura Imóveis"
+detailed description: "Pintura interior e exterior de imóveis"
+activity area: "Construção###"
+proficiency degrees: 0-5, from 0 for "really bad" to 5 for "master at painting"
+</t>
+  </si>
+  <si>
+    <t>Message "Invalid activity area"</t>
+  </si>
+  <si>
+    <t>Popup Message "Invalid activity area"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique code: CP-05
+brief description: "Pintura Imóveis"
+detailed description: "Pintura interior e exterior de imóveis"
+activity area: "Construção"
+proficiency degrees: 0-##, from 0 for "really bad" to ## for "master at painting"
+</t>
+  </si>
+  <si>
+    <t>Message "Invalid proficiency degrees"</t>
+  </si>
+  <si>
+    <t>Popup Message "Invalid proficiency degrees"</t>
+  </si>
+  <si>
+    <t>Valid unique code
+Valid brief description
+Valid detailed description
+Valid activity area
+Invalid proficiency degrees</t>
+  </si>
+  <si>
+    <t>TC_UC7_001</t>
+  </si>
+  <si>
+    <t>TC_UC7_002</t>
+  </si>
+  <si>
+    <t>TC_UC7_003</t>
+  </si>
+  <si>
+    <t>TC_UC7_004</t>
+  </si>
+  <si>
+    <t>TC_UC7_005</t>
+  </si>
+  <si>
+    <t>TC_UC7_006</t>
+  </si>
+  <si>
+    <t>Select tasks to publish
+valid announce period
+valid application period
+valid serialization period
+valid serialization scheme</t>
+  </si>
+  <si>
+    <t>Check "Publicar tarefa" functionality</t>
+  </si>
+  <si>
+    <t>1. Select task to publish
+2. Enter valid announce period
+3. Enter valid application period
+4. Enter valid serialization period
+5. Enter valid serialization scheme
+6. Click publish button</t>
+  </si>
+  <si>
+    <t>1. Enter valid unique code
+2. Enter valid brief description
+3. Enter valid detailed description
+4. Enter valid activity area
+5. Enter valid proficiency degrees
+6. Click register button</t>
+  </si>
+  <si>
+    <t>1. Enter an existant  unique code
+2. Enter valid brief description
+3. Enter valid detailed description
+4. Enter valid activity area
+5. Enter valid proficiency degrees
+6. Click register button</t>
+  </si>
+  <si>
+    <t>1. Enter invalid unique code
+2. Enter valid brief description
+3. Enter valid detailed description
+4. Enter valid activity area
+5. Enter valid proficiency degrees
+6. Click register button</t>
+  </si>
+  <si>
+    <t>1. Enter valid unique code
+2. Enter invalid brief description
+3. Enter valid detailed description
+4. Enter valid activity area
+5. Enter valid proficiency degrees
+6. Click register button</t>
+  </si>
+  <si>
+    <t>1. Enter valid unique code
+2. Enter valid brief description
+3. Enter invalid detailed description
+4. Enter valid activity area
+5. Enter valid proficiency degrees
+6. Click register button</t>
+  </si>
+  <si>
+    <t>1. Enter valid unique code
+2. Enter valid brief description
+3. Enter valid detailed description
+4. Enter valid activity area
+5. Enter invalid proficiency degrees
+6. Click register button</t>
+  </si>
+  <si>
+    <t>task selected: "Reparação Carros GNR"
+announce period: "01/02/2021" to "28/02/2021"
+application period: "01/02/2021" to "28/02/2021"
+serialization period: "01/03/2021" to "15/03/2021"
+serialization scheme: regular</t>
+  </si>
+  <si>
+    <t>Message "Task successfully published"</t>
+  </si>
+  <si>
+    <t>Successful publish a task</t>
+  </si>
+  <si>
+    <t>No tasks to select</t>
+  </si>
+  <si>
+    <t>Message "Error: There are no taks to publish"</t>
+  </si>
+  <si>
+    <t>Select tasks to publish
+invalid announce period
+valid application period
+valid serialization period
+valid serialization scheme</t>
+  </si>
+  <si>
+    <t>1. Select task to publish
+2. Enter invalid announce period
+3. Enter valid application period
+4. Enter valid serialization period
+5. Enter valid serialization scheme
+6. Click publish button</t>
+  </si>
+  <si>
+    <t>task selected: "Reparação Carros GNR"
+announce period: "31/02/2021" to "28/02/2021"
+application period: "01/02/2021" to "28/02/2021"
+serialization period: "01/03/2021" to "15/03/2021"
+serialization scheme: regular</t>
+  </si>
+  <si>
+    <t>Message "Invalid annouce period"</t>
+  </si>
+  <si>
+    <t>1. Select task to publish
+2. Enter valid announce period
+3. Enter invalid application period
+4. Enter valid serialization period
+5. Enter valid serialization scheme
+6. Click publish button</t>
+  </si>
+  <si>
+    <t>task selected: "Reparação Carros GNR"
+announce period: "01/02/2021" to "28/02/2021"
+application period: "31/02/2021" to "28/02/2021"
+serialization period: "01/03/2021" to "15/03/2021"
+serialization scheme: regular</t>
+  </si>
+  <si>
+    <t>Message "Invalid application period"</t>
+  </si>
+  <si>
+    <t>1. Select task to publish
+2. Enter valid announce period
+3. Enter valid application period
+4. Enter invalid serialization period
+5. Enter valid serialization scheme
+6. Click publish button</t>
+  </si>
+  <si>
+    <t>task selected: "Reparação Carros GNR"
+announce period: "01/02/2021" to "28/02/2021"
+application period: "01/02/2021" to "28/02/2021"
+serialization period: "16/03/2021" to "15/03/2021"
+serialization scheme: regular</t>
+  </si>
+  <si>
+    <t>Message "Invalid serialization period"</t>
+  </si>
+  <si>
+    <t>1. Select task to publish
+2. Enter valid announce period
+3. Enter valid application period
+4. Enter valid serialization period
+5. Enter invalid serialization scheme
+6. Click publish button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">task selected: "Reparação Carros GNR"
+announce period: "01/02/2021" to "28/02/2021"
+application period: "01/02/2021" to "28/02/2021"
+serialization period: "01/03/2021" to "15/03/2021"
+serialization scheme: </t>
+  </si>
+  <si>
+    <t>Message "Invalid serialization scheme, must choose one"</t>
+  </si>
+  <si>
+    <t>Check "Especificar competência técnica" functionality</t>
   </si>
 </sst>
 </file>
@@ -193,13 +500,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,9 +827,11 @@
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -524,8 +839,11 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -533,8 +851,11 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -542,8 +863,11 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -551,8 +875,11 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -560,8 +887,11 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -569,15 +899,21 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -593,190 +929,283 @@
       <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="179.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="129" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="C16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
@@ -790,12 +1219,381 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="6" width="27.28515625" customWidth="1"/>
+    <col min="7" max="8" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update Test Scenarios - Julio.xlsx
</commit_message>
<xml_diff>
--- a/Análise/Test Scenarios - Julio.xlsx
+++ b/Análise/Test Scenarios - Julio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UC 4-Especificar Comp.Técnica " sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="92">
   <si>
     <t>Project Name</t>
   </si>
@@ -117,27 +117,6 @@
     <t>Successful register a technical skill</t>
   </si>
   <si>
-    <t>Already existant unique code
-Valid brief description
-Valid detailed description
-Valid activity area
-Valid proficiency degrees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unique code: CP-01
-brief description: "Reparação Automóvel"
-detailed description: "Reparação mecánica automóvel, mecánica geral"
-activity area: "Mecánica"
-proficiency degrees: 0-5, from 0 for "really bad" to 5 for "master at mechanics"
-</t>
-  </si>
-  <si>
-    <t>Message "Unique code already exists"</t>
-  </si>
-  <si>
-    <t>Popup Message "Unique code already exists"</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
@@ -152,9 +131,6 @@
     <t>Message "Invalid unique code"</t>
   </si>
   <si>
-    <t>Popup Message "Invalid unique code"</t>
-  </si>
-  <si>
     <t>TC_UC4_005</t>
   </si>
   <si>
@@ -186,9 +162,6 @@
     <t>Message "Invalid brief description"</t>
   </si>
   <si>
-    <t>Popup Message "Invalid brief description"</t>
-  </si>
-  <si>
     <t xml:space="preserve">unique code: CP-03
 brief description: "Pintura Imóveis"
 detailed description: " "
@@ -200,9 +173,6 @@
     <t>Message "Invalid detailed description"</t>
   </si>
   <si>
-    <t>TC_UC4_007</t>
-  </si>
-  <si>
     <t>Valid unique code
 Valid brief description
 Invalid detailed description
@@ -228,9 +198,6 @@
     <t>Message "Invalid activity area"</t>
   </si>
   <si>
-    <t>Popup Message "Invalid activity area"</t>
-  </si>
-  <si>
     <t xml:space="preserve">unique code: CP-05
 brief description: "Pintura Imóveis"
 detailed description: "Pintura interior e exterior de imóveis"
@@ -242,9 +209,6 @@
     <t>Message "Invalid proficiency degrees"</t>
   </si>
   <si>
-    <t>Popup Message "Invalid proficiency degrees"</t>
-  </si>
-  <si>
     <t>Valid unique code
 Valid brief description
 Valid detailed description
@@ -296,14 +260,6 @@
 6. Click register button</t>
   </si>
   <si>
-    <t>1. Enter an existant  unique code
-2. Enter valid brief description
-3. Enter valid detailed description
-4. Enter valid activity area
-5. Enter valid proficiency degrees
-6. Click register button</t>
-  </si>
-  <si>
     <t>1. Enter invalid unique code
 2. Enter valid brief description
 3. Enter valid detailed description
@@ -435,6 +391,52 @@
   </si>
   <si>
     <t>Check "Especificar competência técnica" functionality</t>
+  </si>
+  <si>
+    <t>InvalidUniqueCodeException</t>
+  </si>
+  <si>
+    <t>InvalidBriefDescriptionException</t>
+  </si>
+  <si>
+    <t>InvalidDetailedDescriptionException</t>
+  </si>
+  <si>
+    <t>InvalidActivityAreaException</t>
+  </si>
+  <si>
+    <t>InvalidProficiencyDegreesException</t>
+  </si>
+  <si>
+    <t>InvalidPeriodDataException</t>
+  </si>
+  <si>
+    <t>InvalidSerializationSchemeException</t>
+  </si>
+  <si>
+    <t>Select tasks to publish
+valid announce period
+invalid application period
+valid serialization period
+valid serialization scheme</t>
+  </si>
+  <si>
+    <t>Select tasks to publish
+valid announce period
+valid application period
+invalid serialization period
+valid serialization scheme</t>
+  </si>
+  <si>
+    <t>Select tasks to publish
+valid announce period
+valid application period
+valid serialization period
+invalid serialization scheme</t>
+  </si>
+  <si>
+    <t>Must have created tasks
+Test Data</t>
   </si>
 </sst>
 </file>
@@ -457,7 +459,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,6 +470,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -500,7 +508,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -511,6 +519,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -816,22 +833,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="7" width="27.42578125" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -841,9 +858,8 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -853,9 +869,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -865,9 +880,8 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -877,9 +891,8 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -889,9 +902,8 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -901,9 +913,8 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
@@ -911,9 +922,8 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -935,37 +945,31 @@
       <c r="G8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -982,16 +986,13 @@
         <v>25</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -999,51 +1000,45 @@
         <v>26</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1065,11 +1060,8 @@
       <c r="G13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="179.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" ht="179.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1080,22 +1072,19 @@
         <v>31</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1106,22 +1095,19 @@
         <v>32</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1129,25 +1115,22 @@
         <v>29</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -1157,9 +1140,8 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1167,50 +1149,44 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1221,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,7 +1297,7 @@
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1343,22 +1319,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -1367,22 +1343,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H10" s="2"/>
     </row>
@@ -1391,22 +1367,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>75</v>
+        <v>54</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -1415,46 +1391,46 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>13</v>
+        <v>91</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="H13" s="4"/>
     </row>
@@ -1463,22 +1439,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H14" s="4"/>
     </row>
@@ -1487,22 +1463,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="G15" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="H15" s="4"/>
     </row>
@@ -1511,22 +1487,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>76</v>
+        <v>64</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H16" s="4"/>
     </row>
@@ -1535,7 +1511,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1549,20 +1525,20 @@
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>34</v>
+      <c r="C18" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H18" s="4"/>
     </row>

</xml_diff>